<commit_message>
Testing on results with automation for pathway methodology. Initial stage, needs better asset definition
</commit_message>
<xml_diff>
--- a/Data/Case_Study/MEX/Results/results_analysis.xlsx
+++ b/Data/Case_Study/MEX/Results/results_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laorie4253/Documents/DPhil-local/year_4/STEVFNs/Data/Case_Study/MEX/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D64CB2A9-F25D-CE45-8BBF-4E59A3780AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{86C47E05-BE61-BA4B-8444-2A941A24FF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" activeTab="1" xr2:uid="{7CF65EC3-B632-544E-8C7F-2BCBF0899D81}"/>
+    <workbookView xWindow="160" yWindow="900" windowWidth="28500" windowHeight="16880" xr2:uid="{7CF65EC3-B632-544E-8C7F-2BCBF0899D81}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
   <si>
     <t>country_1</t>
   </si>
@@ -86,19 +86,31 @@
     <t>PV</t>
   </si>
   <si>
-    <t>Max</t>
+    <t>Emissions (MtCO2e/y)</t>
   </si>
   <si>
-    <t>Min</t>
+    <t>Year</t>
   </si>
   <si>
-    <t>Cummulative installed capacity</t>
+    <t>Emission reduction constraints MEX</t>
   </si>
   <si>
-    <t>MEX</t>
+    <t>Faster initial efforts</t>
   </si>
   <si>
-    <t>Emissions (MtCO2e/y)</t>
+    <t>Slower initial efforts</t>
+  </si>
+  <si>
+    <t>Linear reduction (base scenario)</t>
+  </si>
+  <si>
+    <t>Kmax</t>
+  </si>
+  <si>
+    <t>Kmin</t>
+  </si>
+  <si>
+    <t>Kex</t>
   </si>
 </sst>
 </file>
@@ -660,69 +672,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>MEX initial</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> case study plot testing</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11529510138666295"/>
+          <c:y val="3.9366620557565436E-2"/>
+          <c:w val="0.84686812378541176"/>
+          <c:h val="0.7589713236858906"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -735,16 +697,17 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Max</c:v>
+                  <c:v>Kmax</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="sq">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -822,7 +785,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Min</c:v>
+                  <c:v>Kmin</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -832,6 +795,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -909,7 +873,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cummulative installed capacity</c:v>
+                  <c:v>Kex</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1019,6 +983,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1041,14 +1060,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1081,6 +1100,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Total Installed PV capacity (GWp)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1103,14 +1177,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1132,6 +1206,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28776717069658325"/>
+          <c:y val="0.92847334539263671"/>
+          <c:w val="0.38336314155420836"/>
+          <c:h val="6.4769897850606509E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1145,14 +1229,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -1192,7 +1276,1263 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr b="0" i="0">
+          <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11529510138666295"/>
+          <c:y val="3.9366620557565436E-2"/>
+          <c:w val="0.84686812378541176"/>
+          <c:h val="0.7589713236858906"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$U$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kmax</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$N$4:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$U$4:$U$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.893000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D774-0244-9D16-AE74C8E6594D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kmin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$N$4:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$V$4:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.893000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D774-0244-9D16-AE74C8E6594D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>results!$W$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kex</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>results!$N$4:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>results!$W$4:$W$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10.893000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D774-0244-9D16-AE74C8E6594D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="520514863"/>
+        <c:axId val="1344631920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="520514863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1344631920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1344631920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Total Installed PV capacity (GWp)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="520514863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28776717069658325"/>
+          <c:y val="0.92847334539263671"/>
+          <c:w val="0.38336314155420836"/>
+          <c:h val="6.4769897850606509E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="0" i="0">
+          <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10967506608175306"/>
+          <c:y val="3.8216932185802355E-2"/>
+          <c:w val="0.85640871831253029"/>
+          <c:h val="0.78200910984781613"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 budget reduction'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear reduction (base scenario)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CO2 budget reduction'!$A$4:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CO2 budget reduction'!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACD7-5E43-8389-50EBD9B0A3EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 budget reduction'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Slower initial efforts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CO2 budget reduction'!$A$4:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CO2 budget reduction'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ACD7-5E43-8389-50EBD9B0A3EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CO2 budget reduction'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Faster initial efforts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CO2 budget reduction'!$A$4:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CO2 budget reduction'!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ACD7-5E43-8389-50EBD9B0A3EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="415770431"/>
+        <c:axId val="619661903"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="415770431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1300"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619661903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="619661903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1300"/>
+                  <a:t>Power sector emissions (MtCO</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="800"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1300"/>
+                  <a:t>e / year)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="415770431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.8920606601248897E-2"/>
+          <c:y val="0.93717924272918796"/>
+          <c:w val="0.86476472778101665"/>
+          <c:h val="5.7315066558384239E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="0" i="0">
+          <a:latin typeface="Arial Nova Light" panose="020B0304020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1245,7 +2585,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1766,14 +4218,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1782,6 +4234,85 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{597FB112-1E75-34CC-C556-15D6FEC2B131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE444F85-0D17-2945-ADFD-A36EB3E1DC91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D22479A1-F35C-7CD5-B5E4-84D2EA128978}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2119,15 +4650,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673A9E79-8E3E-164F-884B-EAC0B16599C6}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +4690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2176,7 +4707,7 @@
         <v>130.31472289999999</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2193,16 +4724,25 @@
         <v>57.31427274</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="U3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2234,8 +4774,17 @@
       <c r="Q4">
         <v>6.6950000000000003</v>
       </c>
+      <c r="U4">
+        <v>10.893000000000001</v>
+      </c>
+      <c r="V4">
+        <v>10.893000000000001</v>
+      </c>
+      <c r="W4">
+        <v>10.893000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2267,8 +4816,17 @@
         <f>77.641318874738+J20</f>
         <v>84.336318874737998</v>
       </c>
+      <c r="U5">
+        <v>100</v>
+      </c>
+      <c r="V5">
+        <v>60</v>
+      </c>
+      <c r="W5">
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2300,8 +4858,17 @@
         <f>J11+45.9784122827874</f>
         <v>130.31472290278742</v>
       </c>
+      <c r="U6">
+        <v>155</v>
+      </c>
+      <c r="V6">
+        <v>105</v>
+      </c>
+      <c r="W6">
+        <v>130</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2332,8 +4899,17 @@
         <f>45.97841226+J2</f>
         <v>176.29313515999999</v>
       </c>
+      <c r="U7">
+        <v>176</v>
+      </c>
+      <c r="V7">
+        <v>176</v>
+      </c>
+      <c r="W7">
+        <v>176</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2350,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2367,7 +4943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2384,7 +4960,7 @@
         <v>46.2074085</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2401,7 +4977,7 @@
         <v>84.336310620000006</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2418,7 +4994,7 @@
         <v>32.154636369999999</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2435,7 +5011,7 @@
         <v>45.978412282787403</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2452,7 +5028,7 @@
         <v>25.159636359324001</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2469,7 +5045,7 @@
         <v>153.69705188127099</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2701,55 +5277,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315E65C2-197E-F84C-BCD3-F24540A0ADCC}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2020</v>
-      </c>
-      <c r="B2">
-        <v>119.666581913828</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2025</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>2030</v>
       </c>
-      <c r="B3">
-        <v>79.777721275885341</v>
-      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>2040</v>
       </c>
-      <c r="B4">
-        <v>39.888860637942678</v>
-      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>2050</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2055</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>